<commit_message>
Update Section Properties ITERATION012.xlsx
</commit_message>
<xml_diff>
--- a/src/Section Properties ITERATION012.xlsx
+++ b/src/Section Properties ITERATION012.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\y544q894\Documents\GitHub\structures-calc\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4440F6C7-E6AF-47CD-8F8D-31FE789BAF59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F62EBB9-A9B1-4499-8023-32D76250C8C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -428,6 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BB39"/>
+  <dimension ref="A1:BB51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AZ30" sqref="AZ30:BB30"/>
+      <selection activeCell="D18" sqref="D18:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5845,6 +5846,46 @@
       <c r="U39" s="7"/>
       <c r="V39" s="7"/>
     </row>
+    <row r="47" spans="17:22" x14ac:dyDescent="0.25">
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="9"/>
+      <c r="U47" s="9"/>
+      <c r="V47" s="9"/>
+    </row>
+    <row r="48" spans="17:22" x14ac:dyDescent="0.25">
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="9"/>
+      <c r="V48" s="9"/>
+    </row>
+    <row r="49" spans="17:22" x14ac:dyDescent="0.25">
+      <c r="Q49" s="9"/>
+      <c r="R49" s="9"/>
+      <c r="S49" s="9"/>
+      <c r="T49" s="9"/>
+      <c r="U49" s="9"/>
+      <c r="V49" s="9"/>
+    </row>
+    <row r="50" spans="17:22" x14ac:dyDescent="0.25">
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="9"/>
+      <c r="V50" s="9"/>
+    </row>
+    <row r="51" spans="17:22" x14ac:dyDescent="0.25">
+      <c r="Q51" s="9"/>
+      <c r="R51" s="9"/>
+      <c r="S51" s="9"/>
+      <c r="T51" s="9"/>
+      <c r="U51" s="9"/>
+      <c r="V51" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="Q37:V39"/>

</xml_diff>